<commit_message>
* En el parser desagregar la información de la columna modules. Y poner: “standard modules” y “modules”.
* Mejorar el trabajo de las variables globales:

o Las variables que están dentro de un módulo NO SERÁN VARIABLES GLOBALES. Es decir, no pueden estar en la lista general de variables. Sino que deben ser “atributos” de la clase que representa al módulo.

o En la lista general de variables deberán estar:

* Las variables que están definidas fuera del main(), en el archivo que contiene el main().
</commit_message>
<xml_diff>
--- a/compilador2/Lote de pruebas/summary.xlsx
+++ b/compilador2/Lote de pruebas/summary.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toto\Projects\Proyecto Nacho Cassol\Proyecto-Parser-C\compilador2\Lote de pruebas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="23715" windowHeight="9780"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Case</t>
   </si>
@@ -39,27 +44,18 @@
     <t>WAV maker</t>
   </si>
   <si>
-    <t>Kevin Karplus</t>
-  </si>
-  <si>
     <t>author</t>
   </si>
   <si>
     <t>LightBulbs</t>
   </si>
   <si>
-    <t>Tomas Vilaboa</t>
-  </si>
-  <si>
     <t>BallotBoxes</t>
   </si>
   <si>
     <t>University</t>
   </si>
   <si>
-    <t>Franco Testori</t>
-  </si>
-  <si>
     <t>AssemblyLine</t>
   </si>
   <si>
@@ -75,18 +71,59 @@
     <t>BankSimulation</t>
   </si>
   <si>
-    <t>internet</t>
-  </si>
-  <si>
     <t>Calculator</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>internet - TV</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>internet - FT</t>
+  </si>
+  <si>
+    <t>functions</t>
+  </si>
+  <si>
+    <t>adt's</t>
+  </si>
+  <si>
+    <t>vars</t>
+  </si>
+  <si>
+    <t>modules</t>
+  </si>
+  <si>
+    <t>CCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Supuse q vars se refiere a los #define y no a las variables globales, igual esta todo en el output</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -102,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,27 +162,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,12 +183,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -203,7 +233,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,7 +268,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,275 +477,449 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H13"/>
+  <dimension ref="A3:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1">
         <v>341</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3</v>
+      </c>
+      <c r="J4" s="1">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1">
+        <v>25</v>
+      </c>
+      <c r="L4" s="3">
         <v>41619</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1">
         <v>295</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>7</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>8</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="G5" s="1">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>7</v>
+      </c>
+      <c r="K5" s="1">
+        <v>23</v>
+      </c>
+      <c r="L5" s="3">
         <v>41619</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
         <v>73</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="1">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>6</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3</v>
+      </c>
+      <c r="L6" s="3">
         <v>41619</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1">
+        <v>285</v>
+      </c>
+      <c r="E7" s="1">
         <v>9</v>
       </c>
-      <c r="C7" s="1">
-        <v>285</v>
-      </c>
-      <c r="D7" s="1">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>6</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="G7" s="1">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5</v>
+      </c>
+      <c r="K7" s="1">
+        <v>26</v>
+      </c>
+      <c r="L7" s="3">
         <v>41619</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1">
         <v>228</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>6</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>7</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="G8" s="1">
+        <v>17</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1">
+        <v>8</v>
+      </c>
+      <c r="K8" s="1">
+        <v>21</v>
+      </c>
+      <c r="L8" s="3">
         <v>41619</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1">
         <v>162</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>5</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="G9" s="1">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1">
+        <v>10</v>
+      </c>
+      <c r="L9" s="3">
         <v>41621</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1">
         <v>168</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>7</v>
       </c>
-      <c r="E10" s="1">
-        <v>4</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="F10" s="1">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>6</v>
+      </c>
+      <c r="K10" s="1">
+        <v>10</v>
+      </c>
+      <c r="L10" s="3">
         <v>41621</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1">
+        <v>282</v>
+      </c>
+      <c r="E11" s="1">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1">
+        <v>14</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>7</v>
+      </c>
+      <c r="K11" s="1">
         <v>17</v>
       </c>
-      <c r="C11" s="1">
-        <v>282</v>
-      </c>
-      <c r="D11" s="1">
-        <v>6</v>
-      </c>
-      <c r="E11" s="1">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="L11" s="3">
         <v>41621</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1">
         <v>216</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
         <v>3</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="G12" s="2">
+        <v>6</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>4</v>
+      </c>
+      <c r="K12" s="2">
+        <v>7</v>
+      </c>
+      <c r="L12" s="3">
         <v>41621</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1">
         <v>200</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="G13" s="2">
+        <v>9</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>4</v>
+      </c>
+      <c r="K13" s="2">
+        <v>9</v>
+      </c>
+      <c r="L13" s="3">
         <v>41621</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -730,7 +934,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -742,7 +946,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>